<commit_message>
fix tests for schemas==0.4.7 new uri format
</commit_message>
<xml_diff>
--- a/tests/services/data/pbmc_valid.xlsx
+++ b/tests/services/data/pbmc_valid.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-api-gae/tests/services/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65BB787-327F-9545-ACE9-4324F5867E52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DFE534-32D0-CB44-9919-F429D736260E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="14760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23760" windowHeight="14760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PBMCs" sheetId="1" r:id="rId1"/>
+    <sheet name="shipment" sheetId="1" r:id="rId1"/>
+    <sheet name="aliquots" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -259,7 +260,17 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{71E59CFE-AA76-8142-B2A2-03FE06C23FD8}">
       <text>
         <r>
           <rPr>
@@ -272,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{225E9DBC-E3A9-BA46-A7B7-5B6B08C8CF46}">
       <text>
         <r>
           <rPr>
@@ -285,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{B0B48A2B-6506-9846-978D-9F56864750F6}">
       <text>
         <r>
           <rPr>
@@ -298,7 +309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{1CB30327-1AC0-A04A-9ADC-B22B3C49C9B5}">
       <text>
         <r>
           <rPr>
@@ -311,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{9DB4E4E4-9552-7E4F-B4C7-606BD72B08D8}">
       <text>
         <r>
           <rPr>
@@ -324,7 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{80275666-DDAE-2A4A-A5BA-C940328AF719}">
       <text>
         <r>
           <rPr>
@@ -337,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{D904260A-6685-7640-AC36-F0A46D4C19AB}">
       <text>
         <r>
           <rPr>
@@ -350,7 +361,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{8087506B-BCFA-2B4B-9E2F-DD1D7C2AF187}">
       <text>
         <r>
           <rPr>
@@ -363,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{F8132DDC-108E-554C-ADC4-A527A5933184}">
       <text>
         <r>
           <rPr>
@@ -376,7 +387,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{8CDB0C62-7488-0A49-986B-89A21FB1D694}">
       <text>
         <r>
           <rPr>
@@ -389,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{7288029F-DAF7-3341-A192-9300FF34B56B}">
       <text>
         <r>
           <rPr>
@@ -402,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{0EEB60B7-23C1-4143-85EB-F1EB272F49C4}">
       <text>
         <r>
           <rPr>
@@ -415,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{D62D6863-CB88-C94B-9783-BEF16D0F8EEA}">
       <text>
         <r>
           <rPr>
@@ -428,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{FB7A73F1-797D-5741-83DA-079D906DB76A}">
       <text>
         <r>
           <rPr>
@@ -441,7 +452,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{53948CAA-53F1-594A-942D-B4F788EE28B4}">
       <text>
         <r>
           <rPr>
@@ -454,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{D02E2AE2-3A7A-034B-A336-2AF3CA35B1FA}">
       <text>
         <r>
           <rPr>
@@ -467,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{D3E102DC-A8D7-F74C-8D6D-B407FB535CE9}">
       <text>
         <r>
           <rPr>
@@ -480,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{7622B2CB-7D7B-1F46-92C7-9C3DEA932538}">
       <text>
         <r>
           <rPr>
@@ -493,7 +504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{B84EBF1B-8DCE-624A-A8A3-C5F610F15733}">
       <text>
         <r>
           <rPr>
@@ -506,7 +517,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{1B9BB21E-23FF-FA4F-BC90-532ADB8205BF}">
       <text>
         <r>
           <rPr>
@@ -519,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{7B80F8AE-0376-D941-91FE-4D27909E8DD4}">
       <text>
         <r>
           <rPr>
@@ -532,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{FCBAF0CC-6893-634E-BCB7-6218EED21E97}">
       <text>
         <r>
           <rPr>
@@ -545,7 +556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{CBE7FC9C-0772-7449-9637-1B4338BD258B}">
       <text>
         <r>
           <rPr>
@@ -558,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{B8A82EAD-78B2-014A-BAB5-1262D806D483}">
       <text>
         <r>
           <rPr>
@@ -571,7 +582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{D6D823C3-E025-8C4B-AD66-E5CF96C2E6D8}">
       <text>
         <r>
           <rPr>
@@ -584,7 +595,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{E40FCBF1-69F7-F344-9995-EAB202F1570B}">
       <text>
         <r>
           <rPr>
@@ -602,7 +613,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="75">
   <si>
     <t>#t</t>
   </si>
@@ -928,15 +939,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1275,10 +1286,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA222"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AA212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B20" sqref="A20:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1291,34 +1303,34 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3"/>
-      <c r="AA1" s="3"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
     </row>
     <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1747,7 +1759,7 @@
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1950,618 +1962,50 @@
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
     </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AA21" s="3"/>
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="V22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="W22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="X22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA22" s="2" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="B23">
-        <v>54321</v>
-      </c>
-      <c r="C23">
-        <v>12345</v>
-      </c>
-      <c r="D23">
-        <v>54321</v>
-      </c>
-      <c r="E23">
-        <v>12345</v>
-      </c>
-      <c r="F23">
-        <v>54321</v>
-      </c>
-      <c r="G23">
-        <v>12345</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" s="7">
-        <v>33234</v>
-      </c>
-      <c r="J23" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K23">
-        <v>41193</v>
-      </c>
-      <c r="L23" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M23" t="s">
-        <v>61</v>
-      </c>
-      <c r="N23" t="s">
-        <v>62</v>
-      </c>
-      <c r="O23" t="s">
-        <v>63</v>
-      </c>
-      <c r="P23">
-        <v>100</v>
-      </c>
-      <c r="Q23">
-        <v>100</v>
-      </c>
-      <c r="R23" t="s">
-        <v>64</v>
-      </c>
-      <c r="S23">
-        <v>10</v>
-      </c>
-      <c r="T23" t="s">
-        <v>65</v>
-      </c>
-      <c r="U23" t="s">
-        <v>66</v>
-      </c>
-      <c r="V23">
-        <v>123</v>
-      </c>
-      <c r="W23">
-        <v>122</v>
-      </c>
-      <c r="X23">
-        <v>100</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z23" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA23" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24">
-        <v>54321</v>
-      </c>
-      <c r="C24">
-        <v>12345</v>
-      </c>
-      <c r="D24">
-        <v>54321</v>
-      </c>
-      <c r="E24">
-        <v>12345</v>
-      </c>
-      <c r="F24">
-        <v>54321</v>
-      </c>
-      <c r="G24">
-        <v>12345</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" s="7">
-        <v>33234</v>
-      </c>
-      <c r="J24" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K24">
-        <v>41193</v>
-      </c>
-      <c r="L24" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M24" t="s">
-        <v>61</v>
-      </c>
-      <c r="N24" t="s">
-        <v>62</v>
-      </c>
-      <c r="O24" t="s">
-        <v>63</v>
-      </c>
-      <c r="P24">
-        <v>100</v>
-      </c>
-      <c r="Q24">
-        <v>100</v>
-      </c>
-      <c r="R24" t="s">
-        <v>64</v>
-      </c>
-      <c r="S24">
-        <v>10</v>
-      </c>
-      <c r="T24" t="s">
-        <v>65</v>
-      </c>
-      <c r="U24" t="s">
-        <v>67</v>
-      </c>
-      <c r="V24">
-        <v>123</v>
-      </c>
-      <c r="W24">
-        <v>122</v>
-      </c>
-      <c r="X24">
-        <v>100</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>54321</v>
-      </c>
-      <c r="C25">
-        <v>12345</v>
-      </c>
-      <c r="D25">
-        <v>54321</v>
-      </c>
-      <c r="E25">
-        <v>12345</v>
-      </c>
-      <c r="F25">
-        <v>54321</v>
-      </c>
-      <c r="G25">
-        <v>12345</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="7">
-        <v>33234</v>
-      </c>
-      <c r="J25" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K25">
-        <v>41193</v>
-      </c>
-      <c r="L25" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M25" t="s">
-        <v>61</v>
-      </c>
-      <c r="N25" t="s">
-        <v>62</v>
-      </c>
-      <c r="O25" t="s">
-        <v>63</v>
-      </c>
-      <c r="P25">
-        <v>100</v>
-      </c>
-      <c r="Q25">
-        <v>100</v>
-      </c>
-      <c r="R25" t="s">
-        <v>64</v>
-      </c>
-      <c r="S25">
-        <v>10</v>
-      </c>
-      <c r="T25" t="s">
-        <v>65</v>
-      </c>
-      <c r="U25" t="s">
-        <v>68</v>
-      </c>
-      <c r="V25">
-        <v>123</v>
-      </c>
-      <c r="W25">
-        <v>122</v>
-      </c>
-      <c r="X25">
-        <v>100</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
-        <v>54321</v>
-      </c>
-      <c r="C26">
-        <v>12345</v>
-      </c>
-      <c r="D26">
-        <v>54321</v>
-      </c>
-      <c r="E26">
-        <v>12345</v>
-      </c>
-      <c r="F26">
-        <v>54321</v>
-      </c>
-      <c r="G26">
-        <v>12345</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I26" s="7">
-        <v>33234</v>
-      </c>
-      <c r="J26" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K26">
-        <v>41193</v>
-      </c>
-      <c r="L26" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M26" t="s">
-        <v>61</v>
-      </c>
-      <c r="N26" t="s">
-        <v>62</v>
-      </c>
-      <c r="O26" t="s">
-        <v>63</v>
-      </c>
-      <c r="P26">
-        <v>100</v>
-      </c>
-      <c r="Q26">
-        <v>100</v>
-      </c>
-      <c r="R26" t="s">
-        <v>64</v>
-      </c>
-      <c r="S26">
-        <v>10</v>
-      </c>
-      <c r="T26" t="s">
-        <v>65</v>
-      </c>
-      <c r="U26" t="s">
-        <v>69</v>
-      </c>
-      <c r="V26">
-        <v>123</v>
-      </c>
-      <c r="W26">
-        <v>122</v>
-      </c>
-      <c r="X26">
-        <v>100</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z26" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA26" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-      <c r="B27">
-        <v>54321</v>
-      </c>
-      <c r="C27">
-        <v>12345</v>
-      </c>
-      <c r="D27">
-        <v>54321</v>
-      </c>
-      <c r="E27">
-        <v>12345</v>
-      </c>
-      <c r="F27">
-        <v>54321</v>
-      </c>
-      <c r="G27">
-        <v>12345</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I27" s="7">
-        <v>33234</v>
-      </c>
-      <c r="J27" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K27">
-        <v>41193</v>
-      </c>
-      <c r="L27" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M27" t="s">
-        <v>61</v>
-      </c>
-      <c r="N27" t="s">
-        <v>62</v>
-      </c>
-      <c r="O27" t="s">
-        <v>63</v>
-      </c>
-      <c r="P27">
-        <v>100</v>
-      </c>
-      <c r="Q27">
-        <v>100</v>
-      </c>
-      <c r="R27" t="s">
-        <v>64</v>
-      </c>
-      <c r="S27">
-        <v>10</v>
-      </c>
-      <c r="T27" t="s">
-        <v>65</v>
-      </c>
-      <c r="U27" t="s">
-        <v>70</v>
-      </c>
-      <c r="V27">
-        <v>123</v>
-      </c>
-      <c r="W27">
-        <v>122</v>
-      </c>
-      <c r="X27">
-        <v>100</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA27" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
-      <c r="B28">
-        <v>54321</v>
-      </c>
-      <c r="C28">
-        <v>12345</v>
-      </c>
-      <c r="D28">
-        <v>54321</v>
-      </c>
-      <c r="E28">
-        <v>12345</v>
-      </c>
-      <c r="F28">
-        <v>54321</v>
-      </c>
-      <c r="G28">
-        <v>12345</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I28" s="7">
-        <v>33234</v>
-      </c>
-      <c r="J28" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="K28">
-        <v>41193</v>
-      </c>
-      <c r="L28" s="6">
-        <v>0.42430555555555555</v>
-      </c>
-      <c r="M28" t="s">
-        <v>61</v>
-      </c>
-      <c r="N28" t="s">
-        <v>62</v>
-      </c>
-      <c r="O28" t="s">
-        <v>63</v>
-      </c>
-      <c r="P28">
-        <v>100</v>
-      </c>
-      <c r="Q28">
-        <v>100</v>
-      </c>
-      <c r="R28" t="s">
-        <v>64</v>
-      </c>
-      <c r="S28">
-        <v>10</v>
-      </c>
-      <c r="T28" t="s">
-        <v>65</v>
-      </c>
-      <c r="U28" t="s">
-        <v>71</v>
-      </c>
-      <c r="V28">
-        <v>123</v>
-      </c>
-      <c r="W28">
-        <v>122</v>
-      </c>
-      <c r="X28">
-        <v>100</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>73</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -3483,63 +2927,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A217" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A218" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A219" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A220" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A221" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A222" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="B1:AA1"/>
-    <mergeCell ref="B21:U21"/>
-    <mergeCell ref="V21:AA21"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{F3E6FE57-72BC-A740-8715-EFC67E4B4A18}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
@@ -3552,33 +2944,1668 @@
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14" xr:uid="{9BC69022-A0AD-C645-82ED-2DA1E8EE9692}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K23:K222 I23:I222" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>AND(ISNUMBER(I23:I222),LEFT(CELL("format",I23:I222),1)="D")</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K20:K212 I20:I212" xr:uid="{00000000-0002-0000-0000-000004000000}">
+      <formula1>AND(ISNUMBER(I20:I219),LEFT(CELL("format",I20:I219),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L23:L222 J23:J222" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L20:L212 J20:J212" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N23:N222" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N20:N212" xr:uid="{00000000-0002-0000-0000-000008000000}">
       <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O23:O222" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O20:O212" xr:uid="{00000000-0002-0000-0000-000009000000}">
       <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R23:R222" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R20:R212" xr:uid="{00000000-0002-0000-0000-00000A000000}">
       <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y20:Y212" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z23:Z222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z20:Z212" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA29:AA222" xr:uid="{00000000-0002-0000-0000-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA20:AA212" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA23:AA28" xr:uid="{984A6193-A151-A644-8F31-8366A7AFC467}">
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F096212-B8F8-8645-90B3-5518361EA01E}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:AA202"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B20" sqref="A1:XFD20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>54321</v>
+      </c>
+      <c r="C3">
+        <v>12345</v>
+      </c>
+      <c r="D3">
+        <v>54321</v>
+      </c>
+      <c r="E3">
+        <v>12345</v>
+      </c>
+      <c r="F3">
+        <v>54321</v>
+      </c>
+      <c r="G3">
+        <v>12345</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K3">
+        <v>41193</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>62</v>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3" t="s">
+        <v>64</v>
+      </c>
+      <c r="S3">
+        <v>10</v>
+      </c>
+      <c r="T3" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3">
+        <v>123</v>
+      </c>
+      <c r="W3">
+        <v>122</v>
+      </c>
+      <c r="X3">
+        <v>100</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>54321</v>
+      </c>
+      <c r="C4">
+        <v>12345</v>
+      </c>
+      <c r="D4">
+        <v>54321</v>
+      </c>
+      <c r="E4">
+        <v>12345</v>
+      </c>
+      <c r="F4">
+        <v>54321</v>
+      </c>
+      <c r="G4">
+        <v>12345</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K4">
+        <v>41193</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O4" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4">
+        <v>10</v>
+      </c>
+      <c r="T4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4">
+        <v>123</v>
+      </c>
+      <c r="W4">
+        <v>122</v>
+      </c>
+      <c r="X4">
+        <v>100</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>54321</v>
+      </c>
+      <c r="C5">
+        <v>12345</v>
+      </c>
+      <c r="D5">
+        <v>54321</v>
+      </c>
+      <c r="E5">
+        <v>12345</v>
+      </c>
+      <c r="F5">
+        <v>54321</v>
+      </c>
+      <c r="G5">
+        <v>12345</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K5">
+        <v>41193</v>
+      </c>
+      <c r="L5" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>62</v>
+      </c>
+      <c r="O5" t="s">
+        <v>63</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5" t="s">
+        <v>64</v>
+      </c>
+      <c r="S5">
+        <v>10</v>
+      </c>
+      <c r="T5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" t="s">
+        <v>68</v>
+      </c>
+      <c r="V5">
+        <v>123</v>
+      </c>
+      <c r="W5">
+        <v>122</v>
+      </c>
+      <c r="X5">
+        <v>100</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>54321</v>
+      </c>
+      <c r="C6">
+        <v>12345</v>
+      </c>
+      <c r="D6">
+        <v>54321</v>
+      </c>
+      <c r="E6">
+        <v>12345</v>
+      </c>
+      <c r="F6">
+        <v>54321</v>
+      </c>
+      <c r="G6">
+        <v>12345</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K6">
+        <v>41193</v>
+      </c>
+      <c r="L6" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6">
+        <v>10</v>
+      </c>
+      <c r="T6" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" t="s">
+        <v>69</v>
+      </c>
+      <c r="V6">
+        <v>123</v>
+      </c>
+      <c r="W6">
+        <v>122</v>
+      </c>
+      <c r="X6">
+        <v>100</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7">
+        <v>54321</v>
+      </c>
+      <c r="C7">
+        <v>12345</v>
+      </c>
+      <c r="D7">
+        <v>54321</v>
+      </c>
+      <c r="E7">
+        <v>12345</v>
+      </c>
+      <c r="F7">
+        <v>54321</v>
+      </c>
+      <c r="G7">
+        <v>12345</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K7">
+        <v>41193</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P7">
+        <v>100</v>
+      </c>
+      <c r="Q7">
+        <v>100</v>
+      </c>
+      <c r="R7" t="s">
+        <v>64</v>
+      </c>
+      <c r="S7">
+        <v>10</v>
+      </c>
+      <c r="T7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7">
+        <v>123</v>
+      </c>
+      <c r="W7">
+        <v>122</v>
+      </c>
+      <c r="X7">
+        <v>100</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>54321</v>
+      </c>
+      <c r="C8">
+        <v>12345</v>
+      </c>
+      <c r="D8">
+        <v>54321</v>
+      </c>
+      <c r="E8">
+        <v>12345</v>
+      </c>
+      <c r="F8">
+        <v>54321</v>
+      </c>
+      <c r="G8">
+        <v>12345</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="6">
+        <v>33234</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="K8">
+        <v>41193</v>
+      </c>
+      <c r="L8" s="5">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="M8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8" t="s">
+        <v>64</v>
+      </c>
+      <c r="S8">
+        <v>10</v>
+      </c>
+      <c r="T8" t="s">
+        <v>65</v>
+      </c>
+      <c r="U8" t="s">
+        <v>71</v>
+      </c>
+      <c r="V8">
+        <v>123</v>
+      </c>
+      <c r="W8">
+        <v>122</v>
+      </c>
+      <c r="X8">
+        <v>100</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:U1"/>
+    <mergeCell ref="V1:AA1"/>
+  </mergeCells>
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA8" xr:uid="{F1C69A85-5E53-3344-A5B4-61E17CD8CAB1}">
       <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA9:AA202" xr:uid="{2E778AC8-49C9-2F44-AC60-DBE0A8F348C8}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{5F9E2111-E888-A144-92B3-29BF3F21C820}">
+      <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y202" xr:uid="{D9B9ECAB-8EB3-284C-8269-2AA4D259F44C}">
+      <formula1>"Usable for Assay,Not Usable for Assay,Verifying,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R202" xr:uid="{82DF58DC-30B5-F648-A58F-125ED00B7216}">
+      <formula1>"µL,mL,mg,ng,Vials,Slides,Scrolls,Blocks,ng/µL,cells/ml,N/A,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:O202" xr:uid="{B7318B68-EDBE-1742-BFA6-821A119DB301}">
+      <formula1>"FFPE Block,FFPE Scroll,FFPE Core Punch,Unstained Slide,Frozen Tissue,Sodium Heparin Green-Top Tube,Streck Tube,EDTA Tube,Archival FFPE Block,Archival FFPE Slides,Archival FFPE Core Punch,Archival FFPE Scroll,Frozen Stool,DNA-Preserved Stool,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N202" xr:uid="{F9241F38-D4F5-1342-8A90-95006B344183}">
+      <formula1>"Core Needle Biopsy,Surgical Resection,Endoscopic Biopsy,Punch Biopsy,Plasma,PBMC,Whole Blood,Stool Sample,Bone Marrow Aspirate,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="L3:L202 J3:J202" xr:uid="{50D5E122-54BD-AA4E-A9EB-D7ABEFAB5005}">
+      <formula1>0</formula1>
+      <formula2>0.999305555555555</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="K3:K202 I3:I202" xr:uid="{CAD9ACD2-6EF9-FB49-89F3-892AF85486CC}">
+      <formula1>AND(ISNUMBER(I3:I202),LEFT(CELL("format",I3:I202),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>